<commit_message>
added dev tools and editing sensor info
</commit_message>
<xml_diff>
--- a/text.xlsx
+++ b/text.xlsx
@@ -429,7 +429,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ass</t>
+          <t>test</t>
         </is>
       </c>
     </row>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>787</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>72</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Added comments, formatted to pep and simplified some comparisons
</commit_message>
<xml_diff>
--- a/text.xlsx
+++ b/text.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>604</v>
+        <v>925</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">

</xml_diff>